<commit_message>
Changed card constructor to take Enum, not a character, update tests to use this constructor and all the classes in clueGame package. Siginificant change
</commit_message>
<xml_diff>
--- a/SSAL_ClueLayoutExcel.xlsx
+++ b/SSAL_ClueLayoutExcel.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306\workspace\ClueGameSSALV2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="32100" windowHeight="10320"/>
   </bookViews>
@@ -10,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -602,7 +606,7 @@
   <dimension ref="A1:AT97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y32" sqref="Y32"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>